<commit_message>
overhaul write_to_excel with pandas
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -14,18 +14,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
-    <t>hi</t>
+    <t>ind</t>
   </si>
   <si>
-    <t>a</t>
-  </si>
-  <si>
-    <t>b</t>
-  </si>
-  <si>
-    <t>c</t>
+    <t>ang_vel(limit(asin(protectedDiv(y3, y2), acos(y3, x2)), conditional(x1, conditional(y3, x3)), tan(y3)), cos(sin(x1)), cos(x2), x2)</t>
   </si>
 </sst>
 </file>
@@ -383,123 +377,116 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:Q2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:17">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="1">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="1">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="1">
         <v>3</v>
       </c>
+      <c r="E1" s="1">
+        <v>4</v>
+      </c>
+      <c r="F1" s="1">
+        <v>5</v>
+      </c>
+      <c r="G1" s="1">
+        <v>6</v>
+      </c>
+      <c r="H1" s="1">
+        <v>7</v>
+      </c>
+      <c r="I1" s="1">
+        <v>8</v>
+      </c>
+      <c r="J1" s="1">
+        <v>9.81</v>
+      </c>
+      <c r="K1" s="1">
+        <v>11</v>
+      </c>
+      <c r="L1" s="1">
+        <v>12</v>
+      </c>
+      <c r="M1" s="1">
+        <v>13</v>
+      </c>
+      <c r="N1" s="1">
+        <v>14</v>
+      </c>
+      <c r="O1" s="1">
+        <v>15</v>
+      </c>
+      <c r="P1" s="1">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="1">
+        <v>17</v>
+      </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:17">
+      <c r="A2" t="s">
+        <v>1</v>
+      </c>
       <c r="B2">
-        <v>11</v>
+        <v>-343.33</v>
       </c>
       <c r="C2">
-        <v>21</v>
+        <v>-300.04</v>
       </c>
       <c r="D2">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
-      <c r="B3">
-        <v>12</v>
-      </c>
-      <c r="C3">
-        <v>22</v>
-      </c>
-      <c r="D3">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
-      <c r="B4">
-        <v>31</v>
-      </c>
-      <c r="C4">
-        <v>32</v>
-      </c>
-      <c r="D4">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
-      <c r="B5">
-        <v>11</v>
-      </c>
-      <c r="C5">
-        <v>21</v>
-      </c>
-      <c r="D5">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="B6">
-        <v>12</v>
-      </c>
-      <c r="C6">
-        <v>22</v>
-      </c>
-      <c r="D6">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="B7">
-        <v>31</v>
-      </c>
-      <c r="C7">
-        <v>32</v>
-      </c>
-      <c r="D7">
-        <v>33</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="B8">
-        <v>1</v>
-      </c>
-      <c r="C8">
-        <v>2</v>
-      </c>
-      <c r="D8">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="B9">
-        <v>4</v>
-      </c>
-      <c r="C9">
-        <v>5</v>
-      </c>
-      <c r="D9">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="B10">
-        <v>7</v>
-      </c>
-      <c r="C10">
-        <v>8</v>
-      </c>
-      <c r="D10">
-        <v>9</v>
+        <v>-228.83</v>
+      </c>
+      <c r="E2">
+        <v>-302.76</v>
+      </c>
+      <c r="F2">
+        <v>-303.31</v>
+      </c>
+      <c r="G2">
+        <v>-318.68</v>
+      </c>
+      <c r="H2">
+        <v>-231.48</v>
+      </c>
+      <c r="I2">
+        <v>-177.02</v>
+      </c>
+      <c r="J2">
+        <v>-250.64</v>
+      </c>
+      <c r="K2">
+        <v>-182.02</v>
+      </c>
+      <c r="L2">
+        <v>-201.2</v>
+      </c>
+      <c r="M2">
+        <v>-153.05</v>
+      </c>
+      <c r="N2">
+        <v>-411.3</v>
+      </c>
+      <c r="O2">
+        <v>-466.57</v>
+      </c>
+      <c r="P2">
+        <v>-481.19</v>
+      </c>
+      <c r="Q2">
+        <v>-452.88</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update writing to excel and grav excel
</commit_message>
<xml_diff>
--- a/Book1.xlsx
+++ b/Book1.xlsx
@@ -1,57 +1,51 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
-  <workbookPr defaultThemeVersion="124226"/>
+<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>ind</t>
-  </si>
-  <si>
-    <t>ang_vel(limit(asin(protectedDiv(y3, y2), acos(y3, x2)), conditional(x1, conditional(y3, x3)), tan(y3)), cos(sin(x1)), cos(x2), x2)</t>
-  </si>
-</sst>
-</file>
-
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+  <numFmts count="0"/>
+  <fonts count="3">
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <b val="1"/>
+      <color theme="1"/>
+      <sz val="11"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <b val="1"/>
     </font>
   </fonts>
   <fills count="2">
     <fill>
-      <patternFill patternType="none"/>
+      <patternFill/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -74,21 +68,97 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin"/>
+      <right style="thin"/>
+      <top style="thin"/>
+      <bottom style="thin"/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment horizontal="center" vertical="top"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
 </styleSheet>
 </file>
 
@@ -376,120 +446,314 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:Q2"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1" spans="1:17">
-      <c r="A1" s="1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" s="1">
+    <row r="1">
+      <c r="A1" s="1" t="inlineStr">
+        <is>
+          <t>ind</t>
+        </is>
+      </c>
+      <c r="B1" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="C1" s="1">
+      <c r="C1" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="D1" s="1">
+      <c r="D1" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="E1" s="1">
+      <c r="E1" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="F1" s="1">
+      <c r="F1" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="G1" s="1">
+      <c r="G1" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="H1" s="1">
+      <c r="H1" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="I1" s="1">
+      <c r="I1" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="J1" s="1">
+      <c r="J1" s="1" t="n">
         <v>9.81</v>
       </c>
-      <c r="K1" s="1">
+      <c r="K1" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="L1" s="1">
+      <c r="L1" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="M1" s="1">
+      <c r="M1" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="N1" s="1">
+      <c r="N1" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="O1" s="1">
+      <c r="O1" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="P1" s="1">
+      <c r="P1" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="Q1" s="1">
+      <c r="Q1" s="1" t="n">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:17">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2">
-        <v>-343.33</v>
-      </c>
-      <c r="C2">
-        <v>-300.04</v>
-      </c>
-      <c r="D2">
-        <v>-228.83</v>
-      </c>
-      <c r="E2">
-        <v>-302.76</v>
-      </c>
-      <c r="F2">
-        <v>-303.31</v>
-      </c>
-      <c r="G2">
-        <v>-318.68</v>
-      </c>
-      <c r="H2">
-        <v>-231.48</v>
-      </c>
-      <c r="I2">
-        <v>-177.02</v>
-      </c>
-      <c r="J2">
-        <v>-250.64</v>
-      </c>
-      <c r="K2">
-        <v>-182.02</v>
-      </c>
-      <c r="L2">
-        <v>-201.2</v>
-      </c>
-      <c r="M2">
-        <v>-153.05</v>
-      </c>
-      <c r="N2">
-        <v>-411.3</v>
-      </c>
-      <c r="O2">
-        <v>-466.57</v>
-      </c>
-      <c r="P2">
-        <v>-481.19</v>
-      </c>
-      <c r="Q2">
-        <v>-452.88</v>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ang_vel(limit(asin(protectedDiv(y3, y2), acos(y3, x2)), conditional(x1, conditional(y3, x3)), tan(y3)), cos(sin(x1)), cos(x2), x2)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-1863.44</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1035.52</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-994.45</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-821.1900000000001</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-1322.91</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-2109.39</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-1334.63</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-1129.88</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-1146.39</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-450.94</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-1015.67</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-862.96</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-2025.12</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-2103.14</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-2518.32</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-2614.17</v>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="inlineStr">
+        <is>
+          <t>ang_vel(limit(asin(protectedDiv(y3, y2), acos(y3, x2)), conditional(x1, conditional(y3, x3)), tan(y3)), cos(sin(x1)), cos(x2), x2)</t>
+        </is>
+      </c>
+      <c r="B3" t="n">
+        <v>-1307.97</v>
+      </c>
+      <c r="C3" t="n">
+        <v>-1336.4</v>
+      </c>
+      <c r="D3" t="n">
+        <v>-1165.25</v>
+      </c>
+      <c r="E3" t="n">
+        <v>-1089.9</v>
+      </c>
+      <c r="F3" t="n">
+        <v>-1195.02</v>
+      </c>
+      <c r="G3" t="n">
+        <v>-1346.13</v>
+      </c>
+      <c r="H3" t="n">
+        <v>-1241.05</v>
+      </c>
+      <c r="I3" t="n">
+        <v>-837.1</v>
+      </c>
+      <c r="J3" t="n">
+        <v>-1139.75</v>
+      </c>
+      <c r="K3" t="n">
+        <v>-1072.71</v>
+      </c>
+      <c r="L3" t="n">
+        <v>-917.1799999999999</v>
+      </c>
+      <c r="M3" t="n">
+        <v>-947.85</v>
+      </c>
+      <c r="N3" t="n">
+        <v>-1949.96</v>
+      </c>
+      <c r="O3" t="n">
+        <v>-2289.24</v>
+      </c>
+      <c r="P3" t="n">
+        <v>-2427.33</v>
+      </c>
+      <c r="Q3" t="n">
+        <v>-2673.02</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <sheetPr>
+    <outlinePr summaryBelow="1" summaryRight="1"/>
+    <pageSetUpPr/>
+  </sheetPr>
+  <dimension ref="A1:Q2"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetData>
+    <row r="1">
+      <c r="A1" s="2" t="inlineStr">
+        <is>
+          <t>ind</t>
+        </is>
+      </c>
+      <c r="B1" s="2" t="n">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2" t="n">
+        <v>2</v>
+      </c>
+      <c r="D1" s="2" t="n">
+        <v>3</v>
+      </c>
+      <c r="E1" s="2" t="n">
+        <v>4</v>
+      </c>
+      <c r="F1" s="2" t="n">
+        <v>5</v>
+      </c>
+      <c r="G1" s="2" t="n">
+        <v>6</v>
+      </c>
+      <c r="H1" s="2" t="n">
+        <v>7</v>
+      </c>
+      <c r="I1" s="2" t="n">
+        <v>8</v>
+      </c>
+      <c r="J1" s="2" t="n">
+        <v>9.81</v>
+      </c>
+      <c r="K1" s="2" t="n">
+        <v>11</v>
+      </c>
+      <c r="L1" s="2" t="n">
+        <v>12</v>
+      </c>
+      <c r="M1" s="2" t="n">
+        <v>13</v>
+      </c>
+      <c r="N1" s="2" t="n">
+        <v>14</v>
+      </c>
+      <c r="O1" s="2" t="n">
+        <v>15</v>
+      </c>
+      <c r="P1" s="2" t="n">
+        <v>16</v>
+      </c>
+      <c r="Q1" s="2" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2">
+      <c r="A2" t="inlineStr">
+        <is>
+          <t>ang_vel(limit(asin(protectedDiv(y3, y2), acos(y3, x2)), conditional(x1, conditional(y3, x3)), tan(y3)), cos(sin(x1)), cos(x2), x2)</t>
+        </is>
+      </c>
+      <c r="B2" t="n">
+        <v>-1574.89</v>
+      </c>
+      <c r="C2" t="n">
+        <v>-1364.43</v>
+      </c>
+      <c r="D2" t="n">
+        <v>-1246.63</v>
+      </c>
+      <c r="E2" t="n">
+        <v>-1145.61</v>
+      </c>
+      <c r="F2" t="n">
+        <v>-1339.88</v>
+      </c>
+      <c r="G2" t="n">
+        <v>-1671.42</v>
+      </c>
+      <c r="H2" t="n">
+        <v>-1317.17</v>
+      </c>
+      <c r="I2" t="n">
+        <v>-1091.65</v>
+      </c>
+      <c r="J2" t="n">
+        <v>-1032.3</v>
+      </c>
+      <c r="K2" t="n">
+        <v>-878.47</v>
+      </c>
+      <c r="L2" t="n">
+        <v>-909.39</v>
+      </c>
+      <c r="M2" t="n">
+        <v>-840.4299999999999</v>
+      </c>
+      <c r="N2" t="n">
+        <v>-1836.61</v>
+      </c>
+      <c r="O2" t="n">
+        <v>-2352.45</v>
+      </c>
+      <c r="P2" t="n">
+        <v>-2407.32</v>
+      </c>
+      <c r="Q2" t="n">
+        <v>-2822.27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+</worksheet>
 </file>
</xml_diff>